<commit_message>
- Fixed incorrect NA on rotary-sample fiber in optics BOM.
</commit_message>
<xml_diff>
--- a/optics_BOM.xlsx
+++ b/optics_BOM.xlsx
@@ -54,9 +54,6 @@
     <t>Pigtailed rotary joint</t>
   </si>
   <si>
-    <t>MFP_200/220/900-0.53_1m_FCM-MF1.25</t>
-  </si>
-  <si>
     <t>CLED_560</t>
   </si>
   <si>
@@ -157,6 +154,9 @@
   </si>
   <si>
     <t>BNC cable 0.3m: Photoreciever to acquisition board</t>
+  </si>
+  <si>
+    <t>MFP_200/220/900-0.48_1m_FCM-MF1.25</t>
   </si>
 </sst>
 </file>
@@ -522,7 +522,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,7 +558,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -590,7 +590,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -616,13 +616,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
@@ -632,13 +632,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
@@ -648,13 +648,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
@@ -670,7 +670,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
@@ -680,13 +680,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
         <v>17</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
@@ -696,165 +696,165 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
         <v>21</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12">
         <v>4</v>
       </c>
       <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
         <v>19</v>
-      </c>
-      <c r="D12" t="s">
-        <v>20</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16">
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
         <v>25</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>26</v>
-      </c>
       <c r="D17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19">
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20">
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21">
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- Fixed part number for minicube clamp in optic BOM.
</commit_message>
<xml_diff>
--- a/optics_BOM.xlsx
+++ b/optics_BOM.xlsx
@@ -27,12 +27,6 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>Vendor</t>
-  </si>
-  <si>
-    <t>photoreciever</t>
-  </si>
-  <si>
     <t>Doric</t>
   </si>
   <si>
@@ -96,18 +90,12 @@
     <t>121-3251</t>
   </si>
   <si>
-    <t>CL3/M-P5 Compact Variable Height Clamp, M6 Tapped</t>
-  </si>
-  <si>
     <t>Clamp for photodetector</t>
   </si>
   <si>
     <t>Pillar for photodetector</t>
   </si>
   <si>
-    <t>M6 x 12mm Socket Cap Screw</t>
-  </si>
-  <si>
     <t>TRP14/M Ø12 mm Pedestal Pillar Post</t>
   </si>
   <si>
@@ -126,12 +114,6 @@
     <t>Fiber patchcord: Rotary-sample</t>
   </si>
   <si>
-    <t>M6 - M3 thread adapter (for mounting acquistion board)</t>
-  </si>
-  <si>
-    <t>M6 x 45mm (for minicube clamp)</t>
-  </si>
-  <si>
     <t>468-0133</t>
   </si>
   <si>
@@ -141,22 +123,40 @@
     <t>660-4636</t>
   </si>
   <si>
-    <t>M3 screw 10mm (for mounting acquistion board)</t>
-  </si>
-  <si>
-    <t>M3 spacer 3mm (for mounting acquistion board)</t>
-  </si>
-  <si>
     <t>161-3676</t>
   </si>
   <si>
-    <t>m6 screw 12mm  (for mounting LEDs and photodetectors)</t>
-  </si>
-  <si>
     <t>BNC cable 0.3m: Photoreciever to acquisition board</t>
   </si>
   <si>
     <t>MFP_200/220/900-0.48_1m_FCM-MF1.25</t>
+  </si>
+  <si>
+    <t>Photoreciever</t>
+  </si>
+  <si>
+    <t>M6 - M3 thread adapter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M6 screw 12mm </t>
+  </si>
+  <si>
+    <t>M3 screw 10mm</t>
+  </si>
+  <si>
+    <t>M3 spacer 3mm</t>
+  </si>
+  <si>
+    <t>M6 x 45mm</t>
+  </si>
+  <si>
+    <t>SH6MS12</t>
+  </si>
+  <si>
+    <t>CL3/M Compact Variable Height Clamp, M6 Tapped</t>
+  </si>
+  <si>
+    <t>Supplier</t>
   </si>
 </sst>
 </file>
@@ -166,8 +166,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -201,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -215,6 +223,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,14 +531,14 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58.42578125" customWidth="1"/>
+    <col min="1" max="1" width="51.28515625" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="53.7109375" customWidth="1"/>
+    <col min="3" max="3" width="52.42578125" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
     <col min="5" max="5" width="47.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="19.85546875" customWidth="1"/>
@@ -537,281 +546,281 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
+      <c r="D1" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B12">
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B16">
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G18" s="3"/>
     </row>
@@ -823,10 +832,10 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -837,24 +846,24 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B21">
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- Optics_BOM: Changed fiber connecting LEDs to minicube from 0.22 to 0.48NA.
</commit_message>
<xml_diff>
--- a/optics_BOM.xlsx
+++ b/optics_BOM.xlsx
@@ -51,9 +51,6 @@
     <t>CLED_560</t>
   </si>
   <si>
-    <t>MFP_200/220/LWMJ-0.22_0.3m_FCM-FCM</t>
-  </si>
-  <si>
     <t>MFP_600/630/LWMJ-0.48_0.3m_FCM-FCM</t>
   </si>
   <si>
@@ -157,6 +154,9 @@
   </si>
   <si>
     <t>Supplier</t>
+  </si>
+  <si>
+    <t>MFP_200/220/LWMJ-0.48_0.3m_FCM-FCM</t>
   </si>
 </sst>
 </file>
@@ -531,7 +531,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,18 +556,18 @@
         <v>1</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -625,13 +625,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
         <v>3</v>
@@ -641,13 +641,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
         <v>3</v>
@@ -657,13 +657,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
         <v>3</v>
@@ -679,7 +679,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
         <v>3</v>
@@ -689,13 +689,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
         <v>3</v>
@@ -705,165 +705,165 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12">
         <v>4</v>
       </c>
       <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
         <v>16</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16">
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19">
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20">
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B21">
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>